<commit_message>
trc khi bao cao
</commit_message>
<xml_diff>
--- a/cypress/downloads/_search_store_name.xlsx
+++ b/cypress/downloads/_search_store_name.xlsx
@@ -408,7 +408,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>location</v>
+        <v>name</v>
       </c>
       <c r="B1" t="str">
         <v>contain</v>
@@ -419,10 +419,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>828 sư vạn hạnh phường 13 quận 10 thành phố hồ chí minh</v>
+        <v>na flower</v>
       </c>
       <c r="B2" t="str">
-        <v>sư vạn hạnh</v>
+        <v>na</v>
       </c>
       <c r="C2" t="str">
         <v>passed</v>

</xml_diff>